<commit_message>
Configure the New Web
</commit_message>
<xml_diff>
--- a/regresi_linear.xlsx
+++ b/regresi_linear.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
   <si>
     <t>Buffer pH</t>
   </si>
@@ -34,14 +35,100 @@
   </si>
   <si>
     <t>Volt</t>
+  </si>
+  <si>
+    <t>PH4</t>
+  </si>
+  <si>
+    <t>Suhu</t>
+  </si>
+  <si>
+    <t>SUMMARY OUTPUT</t>
+  </si>
+  <si>
+    <t>Regression Statistics</t>
+  </si>
+  <si>
+    <t>Multiple R</t>
+  </si>
+  <si>
+    <t>R Square</t>
+  </si>
+  <si>
+    <t>Adjusted R Square</t>
+  </si>
+  <si>
+    <t>Standard Error</t>
+  </si>
+  <si>
+    <t>Observations</t>
+  </si>
+  <si>
+    <t>ANOVA</t>
+  </si>
+  <si>
+    <t>Regression</t>
+  </si>
+  <si>
+    <t>Residual</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Intercept</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Significance F</t>
+  </si>
+  <si>
+    <t>Coefficients</t>
+  </si>
+  <si>
+    <t>t Stat</t>
+  </si>
+  <si>
+    <t>P-value</t>
+  </si>
+  <si>
+    <t>Lower 95%</t>
+  </si>
+  <si>
+    <t>Upper 95%</t>
+  </si>
+  <si>
+    <t>Lower 95,0%</t>
+  </si>
+  <si>
+    <t>Upper 95,0%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -57,7 +144,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -65,12 +152,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -250,13 +365,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>2.96</c:v>
+                  <c:v>3.03</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.4900000000000002</c:v>
+                  <c:v>2.6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0699999999999998</c:v>
+                  <c:v>2.27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -448,373 +563,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$C$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Volt</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$B$5:$B$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>4.01</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6.86</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>9.0399999999999991</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$C$5:$C$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>2.96</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.4900000000000002</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.0699999999999998</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E36C-4D0A-86FA-E9FB30C85AE0}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="1912617856"/>
-        <c:axId val="1912618688"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="1912617856"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1912618688"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="1912618688"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1912617856"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1370,536 +1119,20 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>129540</xdr:colOff>
+      <xdr:colOff>335280</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>179070</xdr:rowOff>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>434340</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>179070</xdr:rowOff>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1913,36 +1146,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>45720</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>102870</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>350520</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>102870</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2214,77 +1417,382 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:K7"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B3" s="1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="4"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1">
         <v>1</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="F3" s="1" t="s">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1">
+        <v>65535</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="1">
         <v>2</v>
       </c>
-      <c r="G3" s="1"/>
-      <c r="J3" s="1" t="s">
+      <c r="C12" s="1">
+        <v>0.39646666666666674</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.19823333333333337</v>
+      </c>
+      <c r="E12" s="1" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="F12" s="1" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
+        <v>65535</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="2">
+        <v>2</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.39646666666666674</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="1">
+        <v>4.0060805577072092</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1">
+        <v>65535</v>
+      </c>
+      <c r="E17" s="1" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="F17" s="1">
+        <v>4.0060805577072092</v>
+      </c>
+      <c r="G17" s="1">
+        <v>4.0060805577072092</v>
+      </c>
+      <c r="H17" s="1">
+        <v>4.0060805577072092</v>
+      </c>
+      <c r="I17" s="1">
+        <v>4.0060805577072092</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="1">
+        <v>-0.17428350116188993</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1">
+        <v>65535</v>
+      </c>
+      <c r="E18" s="1" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="F18" s="1">
+        <v>-0.17428350116188993</v>
+      </c>
+      <c r="G18" s="1">
+        <v>-0.17428350116188993</v>
+      </c>
+      <c r="H18" s="1">
+        <v>-0.17428350116188993</v>
+      </c>
+      <c r="I18" s="1">
+        <v>-0.17428350116188993</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="2">
+        <v>-1.3353989155693509E-2</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0</v>
+      </c>
+      <c r="D19" s="2">
+        <v>65535</v>
+      </c>
+      <c r="E19" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="F19" s="2">
+        <v>-1.3353989155693509E-2</v>
+      </c>
+      <c r="G19" s="2">
+        <v>-1.3353989155693509E-2</v>
+      </c>
+      <c r="H19" s="2">
+        <v>-1.3353989155693509E-2</v>
+      </c>
+      <c r="I19" s="2">
+        <v>-1.3353989155693509E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:Q11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="3" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="L3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3" s="5"/>
+      <c r="P3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="1"/>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="Q3" s="5"/>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>0</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="F4" t="s">
+      <c r="L4" t="s">
         <v>0</v>
       </c>
-      <c r="G4" t="s">
+      <c r="M4" t="s">
         <v>4</v>
       </c>
-      <c r="J4" t="s">
+      <c r="P4" t="s">
         <v>0</v>
       </c>
-      <c r="K4" t="s">
+      <c r="Q4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>4.01</v>
       </c>
       <c r="C5">
-        <v>2.96</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+        <v>3.03</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>6.86</v>
       </c>
       <c r="C6">
-        <v>2.4900000000000002</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>9.0399999999999991</v>
       </c>
       <c r="C7">
+        <v>2.27</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="N8" t="s">
+        <v>0</v>
+      </c>
+      <c r="O8" t="s">
+        <v>6</v>
+      </c>
+      <c r="P8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="N9">
+        <v>4.01</v>
+      </c>
+      <c r="O9">
+        <v>26</v>
+      </c>
+      <c r="P9">
+        <v>2.96</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="N10">
+        <v>6.86</v>
+      </c>
+      <c r="O10">
+        <v>24</v>
+      </c>
+      <c r="P10">
+        <v>2.4900000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="N11">
+        <v>9.0399999999999991</v>
+      </c>
+      <c r="O11">
+        <v>27</v>
+      </c>
+      <c r="P11">
         <v>2.0699999999999998</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="B3:C3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="N7:P7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>